<commit_message>
Incorporated new health estimates -also adjusted leisure time to match Draia's definition (18*7 instead of 24*7)
</commit_message>
<xml_diff>
--- a/input/PL/reg_health.xlsx
+++ b/input/PL/reg_health.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyburdett/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pineapple/IdeaProjects/SimPathsEU_JAN/input/PL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{74DADF49-2C46-9D41-80DE-2C7D915282A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40DFA3B6-0F51-4300-BF3A-C5C861AE3B65}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F26EEA6-8C14-454D-BAF9-7F3A84568191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20180" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="124">
   <si>
     <t>Description:</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Constant_VeryGood</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Dgn</t>
   </si>
   <si>
@@ -420,7 +417,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -807,13 +804,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -821,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -829,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -837,7 +834,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -845,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -853,17 +850,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -871,7 +868,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -890,19 +887,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -916,7 +913,7 @@
         <v>13192.580589398955</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -937,19 +934,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D987FF1B-1A34-F74C-BFCD-534EA01B9051}">
-  <dimension ref="A1:BW73"/>
+  <dimension ref="A1:BV73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BW2" sqref="BW2:BW73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="33.6640625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1172,11 +1169,8 @@
       <c r="BV1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BW1" s="2" t="s">
-        <v>95</v>
-      </c>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1400,7 +1394,7 @@
         <v>8.3845124420664531E-6</v>
       </c>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1624,7 +1618,7 @@
         <v>-1.2790177624525648E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1842,7 @@
         <v>9.7035284665638929E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:75">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2072,7 +2066,7 @@
         <v>4.295714425938936E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:75">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -2296,7 +2290,7 @@
         <v>-8.9425298677476338E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:75">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -2520,7 +2514,7 @@
         <v>-6.6007249398807326E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:75">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -2744,7 +2738,7 @@
         <v>-8.5684680128256046E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:75">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2968,7 +2962,7 @@
         <v>-1.0678612492180718E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:75">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -3192,7 +3186,7 @@
         <v>-1.3435908381603996E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:75">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -3416,7 +3410,7 @@
         <v>-8.9510883154968998E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:75">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -3640,7 +3634,7 @@
         <v>-4.6631485131188302E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:75">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -3864,7 +3858,7 @@
         <v>-2.7157685076887586E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:75">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -4088,7 +4082,7 @@
         <v>-1.9087800636316763E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:75">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
@@ -4312,7 +4306,7 @@
         <v>1.9422343795749559E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:75">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -4536,7 +4530,7 @@
         <v>4.094861595811893E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:74">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -4760,7 +4754,7 @@
         <v>-1.0023856945598798E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:74">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -4984,7 +4978,7 @@
         <v>-5.9645674489044683E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:74">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
@@ -5208,7 +5202,7 @@
         <v>-1.4975490457535439E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:74">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -5432,7 +5426,7 @@
         <v>3.1996994018132355E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:74">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -5656,7 +5650,7 @@
         <v>-4.9006662333421579E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:74">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
@@ -5880,7 +5874,7 @@
         <v>-1.5705042921266625E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:74">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -6104,7 +6098,7 @@
         <v>-2.2606923800853338E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:74">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -6328,7 +6322,7 @@
         <v>6.7206571857118537E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:74">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -6552,7 +6546,7 @@
         <v>1.9320136523491786E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:74">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -6776,7 +6770,7 @@
         <v>-7.2906710439951669E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:74">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -7000,7 +6994,7 @@
         <v>-2.2114291755728164E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:74">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -7224,7 +7218,7 @@
         <v>1.7039144933796389E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:74">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -7448,7 +7442,7 @@
         <v>-2.0836291936670911E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:74">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -7672,7 +7666,7 @@
         <v>-2.0767521984875435E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:74">
+    <row r="31" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
@@ -7896,7 +7890,7 @@
         <v>-2.3306256488971398E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:74">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
@@ -8120,7 +8114,7 @@
         <v>-2.4450986617872705E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:74">
+    <row r="33" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>54</v>
       </c>
@@ -8344,7 +8338,7 @@
         <v>-1.0537016189484755E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:74">
+    <row r="34" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -8568,7 +8562,7 @@
         <v>-2.0103214791417252E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:74">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
@@ -8792,7 +8786,7 @@
         <v>1.7280799388461364E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:74">
+    <row r="36" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -9016,7 +9010,7 @@
         <v>-5.8481636571108412E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:74">
+    <row r="37" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -9240,7 +9234,7 @@
         <v>-9.3305946274750129E-6</v>
       </c>
     </row>
-    <row r="38" spans="1:74">
+    <row r="38" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
@@ -9464,7 +9458,7 @@
         <v>-1.4360902626033974E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:74">
+    <row r="39" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>60</v>
       </c>
@@ -9688,7 +9682,7 @@
         <v>-5.5742762409227672E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:74">
+    <row r="40" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -9912,7 +9906,7 @@
         <v>6.6928552242923598E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:74">
+    <row r="41" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
@@ -10136,7 +10130,7 @@
         <v>2.1065005537502256E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:74">
+    <row r="42" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
@@ -10360,7 +10354,7 @@
         <v>-5.9741036708225716E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:74">
+    <row r="43" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>64</v>
       </c>
@@ -10584,7 +10578,7 @@
         <v>-6.4751109558065505E-5</v>
       </c>
     </row>
-    <row r="44" spans="1:74">
+    <row r="44" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -10808,7 +10802,7 @@
         <v>5.961441493008327E-7</v>
       </c>
     </row>
-    <row r="45" spans="1:74">
+    <row r="45" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>66</v>
       </c>
@@ -11032,7 +11026,7 @@
         <v>-1.0794524903055569E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:74">
+    <row r="46" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>67</v>
       </c>
@@ -11256,7 +11250,7 @@
         <v>-1.084900260137416E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:74">
+    <row r="47" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>68</v>
       </c>
@@ -11480,7 +11474,7 @@
         <v>-1.0899506785011863E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:74">
+    <row r="48" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
@@ -11704,7 +11698,7 @@
         <v>-1.0999954788651137E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:74">
+    <row r="49" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>70</v>
       </c>
@@ -11928,7 +11922,7 @@
         <v>-2.8066490693565237E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:74">
+    <row r="50" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>71</v>
       </c>
@@ -12152,7 +12146,7 @@
         <v>-6.2472209808942772E-4</v>
       </c>
     </row>
-    <row r="51" spans="1:74">
+    <row r="51" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
@@ -12376,7 +12370,7 @@
         <v>-1.9598227509087758E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:74">
+    <row r="52" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -12600,7 +12594,7 @@
         <v>-6.2891417266685127E-6</v>
       </c>
     </row>
-    <row r="53" spans="1:74">
+    <row r="53" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>74</v>
       </c>
@@ -12824,7 +12818,7 @@
         <v>-1.4446428482840448E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:74">
+    <row r="54" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>75</v>
       </c>
@@ -13048,7 +13042,7 @@
         <v>-2.2768500051553327E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:74">
+    <row r="55" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>76</v>
       </c>
@@ -13272,7 +13266,7 @@
         <v>-1.4757879787787799E-4</v>
       </c>
     </row>
-    <row r="56" spans="1:74">
+    <row r="56" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>77</v>
       </c>
@@ -13496,7 +13490,7 @@
         <v>6.6281016101589013E-5</v>
       </c>
     </row>
-    <row r="57" spans="1:74">
+    <row r="57" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>78</v>
       </c>
@@ -13720,7 +13714,7 @@
         <v>3.107341222864541E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:74">
+    <row r="58" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>79</v>
       </c>
@@ -13944,7 +13938,7 @@
         <v>-4.5132771302849189E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:74">
+    <row r="59" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>80</v>
       </c>
@@ -14168,7 +14162,7 @@
         <v>-5.5956380111732407E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:74">
+    <row r="60" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
@@ -14392,7 +14386,7 @@
         <v>5.6039427366635544E-6</v>
       </c>
     </row>
-    <row r="61" spans="1:74">
+    <row r="61" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>82</v>
       </c>
@@ -14616,7 +14610,7 @@
         <v>-5.3702384439649496E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:74">
+    <row r="62" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>83</v>
       </c>
@@ -14840,7 +14834,7 @@
         <v>-5.4080110039879614E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:74">
+    <row r="63" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>84</v>
       </c>
@@ -15064,7 +15058,7 @@
         <v>-5.4673378075727058E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:74">
+    <row r="64" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>85</v>
       </c>
@@ -15288,7 +15282,7 @@
         <v>-5.4897047787711928E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:74">
+    <row r="65" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
@@ -15512,7 +15506,7 @@
         <v>-7.8778933344475933E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:74">
+    <row r="66" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>87</v>
       </c>
@@ -15736,7 +15730,7 @@
         <v>-3.1879105921643865E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:74">
+    <row r="67" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>88</v>
       </c>
@@ -15960,7 +15954,7 @@
         <v>-1.4845521636138491E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:74">
+    <row r="68" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>89</v>
       </c>
@@ -16184,7 +16178,7 @@
         <v>-2.8370743739242888E-4</v>
       </c>
     </row>
-    <row r="69" spans="1:74">
+    <row r="69" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>90</v>
       </c>
@@ -16408,7 +16402,7 @@
         <v>-6.0537928596875938E-4</v>
       </c>
     </row>
-    <row r="70" spans="1:74">
+    <row r="70" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>91</v>
       </c>
@@ -16632,7 +16626,7 @@
         <v>-1.4927729418009452E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:74">
+    <row r="71" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>92</v>
       </c>
@@ -16856,7 +16850,7 @@
         <v>-4.3857321462845308E-4</v>
       </c>
     </row>
-    <row r="72" spans="1:74">
+    <row r="72" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>93</v>
       </c>
@@ -17080,7 +17074,7 @@
         <v>6.5407195073386879E-5</v>
       </c>
     </row>
-    <row r="73" spans="1:74">
+    <row r="73" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>94</v>
       </c>
@@ -17311,13 +17305,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -17325,99 +17321,96 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>104</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>105</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>106</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>107</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>108</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>110</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>111</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>112</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>113</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>114</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>115</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>116</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>118</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>120</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>121</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>122</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>123</v>
       </c>
-      <c r="AE1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32">
-      <c r="A2" t="s">
-        <v>96</v>
       </c>
       <c r="B2">
         <v>0.1284783664970732</v>
@@ -17510,9 +17503,9 @@
         <v>-1.0119295585513386E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <v>3.7488743125440295E-2</v>
@@ -17605,9 +17598,9 @@
         <v>-1.5892853410290793E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <v>-3.8334491074713952E-4</v>
@@ -17700,9 +17693,9 @@
         <v>1.6071297443999355E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>4.4570093961561703E-2</v>
@@ -17795,9 +17788,9 @@
         <v>-1.0517091259854376E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6">
         <v>-0.21288447366929097</v>
@@ -17890,9 +17883,9 @@
         <v>-4.0794457840763064E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7">
         <v>-0.36286044837297854</v>
@@ -17985,9 +17978,9 @@
         <v>1.9897477847352212E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8">
         <v>-0.49994184411256626</v>
@@ -18080,9 +18073,9 @@
         <v>4.947281949105669E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:32">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9">
         <v>-0.26213417684943685</v>
@@ -18175,9 +18168,9 @@
         <v>-8.7876303844474496E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10">
         <v>-3.8895436030319322E-2</v>
@@ -18270,9 +18263,9 @@
         <v>-1.6685919692755193E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11">
         <v>2.2488359484194791</v>
@@ -18365,9 +18358,9 @@
         <v>-9.2148308630497014E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12">
         <v>1.9559635602331087</v>
@@ -18460,9 +18453,9 @@
         <v>-9.0550632103783644E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13">
         <v>1.4242139742896991</v>
@@ -18555,9 +18548,9 @@
         <v>-8.876807164860865E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>0.61510998545832007</v>
@@ -18650,9 +18643,9 @@
         <v>-9.9496734182461001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15">
         <v>-9.5901618193934279E-2</v>
@@ -18745,9 +18738,9 @@
         <v>-5.1415108699594974E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16">
         <v>-4.3118894163539619E-3</v>
@@ -18840,9 +18833,9 @@
         <v>-6.6931893039293274E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17">
         <v>-4.1655923345639374E-3</v>
@@ -18935,9 +18928,9 @@
         <v>-3.1458434710124555E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18">
         <v>-8.3675237424668796E-3</v>
@@ -19030,9 +19023,9 @@
         <v>-2.6432605674720291E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>3.0554986293204256</v>
@@ -19125,9 +19118,9 @@
         <v>8.3054988050408764E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B20">
         <v>-0.30980749651543793</v>
@@ -19220,9 +19213,9 @@
         <v>-5.6338260547464417E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B21">
         <v>-8.4942787693746774E-2</v>
@@ -19315,9 +19308,9 @@
         <v>-2.1633533272268522E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22">
         <v>-0.32979643659351687</v>
@@ -19410,9 +19403,9 @@
         <v>2.0864193876174011E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B23">
         <v>0.10519861119949105</v>
@@ -19505,9 +19498,9 @@
         <v>-4.8029089668309688E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B24">
         <v>-2.0464004720107511E-3</v>
@@ -19600,9 +19593,9 @@
         <v>-8.9967105822487945E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25">
         <v>9.5508393160406074E-2</v>
@@ -19695,9 +19688,9 @@
         <v>-1.7219337612428597E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B26">
         <v>7.4843363688279818E-2</v>
@@ -19790,9 +19783,9 @@
         <v>-1.1399722463119513E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B27">
         <v>8.5100358359127739E-3</v>
@@ -19885,9 +19878,9 @@
         <v>-2.0791996004202327E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B28">
         <v>0.18213314893728641</v>
@@ -19980,9 +19973,9 @@
         <v>8.6994691965731235E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B29">
         <v>0.25427383825045052</v>
@@ -20075,9 +20068,9 @@
         <v>7.3291797463296117E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B30">
         <v>-4.2528114629984879</v>

</xml_diff>